<commit_message>
CORRECCION DE FUNCION ADMIN PROJECT
</commit_message>
<xml_diff>
--- a/Cosa para hacer tp fina_P_A.xlsx
+++ b/Cosa para hacer tp fina_P_A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t xml:space="preserve">Estado </t>
   </si>
@@ -228,12 +228,15 @@
   <si>
     <t xml:space="preserve">Estados de item </t>
   </si>
+  <si>
+    <t>MODIFICAR EL ALTA de un ITEM LO DE DE ALTA AL SIN ASIGNAR  "estado SIN ASIGNAR "</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +340,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -365,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -392,6 +401,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,16 +706,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="102.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
@@ -802,49 +812,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
@@ -854,25 +864,25 @@
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>6</v>
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>13</v>
+      <c r="A21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,7 +890,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>13</v>
@@ -891,13 +901,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -905,18 +912,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>13</v>
@@ -925,12 +935,9 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
+    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>40</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>13</v>
@@ -940,109 +947,123 @@
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+      <c r="C39" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="C41" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A49" s="11" t="s">
+      <c r="C45" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
+    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A52" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="12" t="s">
+      <c r="C52" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A53" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="11"/>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="C53" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A54" s="11"/>
+    </row>
+    <row r="56" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="62" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+      <c r="C62" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Modificaciones de crud de usuario, crud de items Crud de proyectos, Modificacion de la raelacion entre items hstorica para la visualizacion coorrecta de la de los items asignados.
</commit_message>
<xml_diff>
--- a/Cosa para hacer tp fina_P_A.xlsx
+++ b/Cosa para hacer tp fina_P_A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t xml:space="preserve">Estado </t>
   </si>
@@ -231,12 +231,27 @@
   <si>
     <t>MODIFICAR EL ALTA de un ITEM LO DE DE ALTA AL SIN ASIGNAR  "estado SIN ASIGNAR "</t>
   </si>
+  <si>
+    <t xml:space="preserve">Alta de usuarioos:  AGREGAR DROPDOWN EN Alta de usuarios para el perfil </t>
+  </si>
+  <si>
+    <t>PRIORIDAD - Priority  Ver como manejar eso</t>
+  </si>
+  <si>
+    <t>hecho(Espacio vacio por ahora )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hecho(se deja sin estado) </t>
+  </si>
+  <si>
+    <t>Alta de Item:  PRIORIDAD - Priority  Ver como manejar eso</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,7 +357,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
@@ -374,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,6 +431,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,17 +737,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.5703125" customWidth="1"/>
+    <col min="1" max="1" width="119.7109375" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -812,18 +843,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -892,8 +923,8 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>13</v>
+      <c r="C23" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,8 +970,8 @@
       <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>13</v>
+      <c r="C31" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,8 +1022,8 @@
       <c r="A41" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>13</v>
+      <c r="C41" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1064,6 +1095,25 @@
         <v>46</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion de alta de usuarios
</commit_message>
<xml_diff>
--- a/Cosa para hacer tp fina_P_A.xlsx
+++ b/Cosa para hacer tp fina_P_A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t xml:space="preserve">Estado </t>
   </si>
@@ -246,6 +246,12 @@
   <si>
     <t>Alta de Item:  PRIORIDAD - Priority  Ver como manejar eso</t>
   </si>
+  <si>
+    <t xml:space="preserve">ARREGLAR ALTA DE USUARIOS </t>
+  </si>
+  <si>
+    <t>no funciona</t>
+  </si>
 </sst>
 </file>
 
@@ -403,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -433,6 +439,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,75 +1052,92 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A52" s="11"/>
     </row>
     <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>13</v>
+      <c r="A53" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="11"/>
     </row>
-    <row r="56" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A55" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A56" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A57" s="11"/>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="65" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="C65" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="C69" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="C71" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>53</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>50</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>